<commit_message>
deleted key for security
</commit_message>
<xml_diff>
--- a/data/raw_data_1203.xlsx
+++ b/data/raw_data_1203.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="raw_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>